<commit_message>
Hoang tich hop them chuc nang QuanLyTrongTai (100%)
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>75%(Chưa làm phần GUI )</t>
+  </si>
+  <si>
+    <t>100% (9/06/2010)</t>
+  </si>
+  <si>
+    <t>100% (8/06/2010)</t>
   </si>
 </sst>
 </file>
@@ -737,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -790,7 +796,9 @@
       <c r="D3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="14"/>
+      <c r="E3" s="14" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="29"/>
@@ -803,7 +811,9 @@
       <c r="D4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="30">
       <c r="A5" s="29"/>
@@ -813,8 +823,12 @@
       <c r="C5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="29"/>

</xml_diff>

<commit_message>
Hoang tich hop chuc nang QuanLyLoaiHang(100%)
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -252,9 +252,6 @@
 trước Deadline</t>
   </si>
   <si>
-    <t>70% (Xong 2/3 Chức năng)</t>
-  </si>
-  <si>
     <t>75%(Chưa làm phần GUI )</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>100% (8/06/2010)</t>
+  </si>
+  <si>
+    <t>70% (Chưa có cn Cập Nhật)</t>
   </si>
 </sst>
 </file>
@@ -794,10 +794,10 @@
         <v>18</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
@@ -809,10 +809,10 @@
         <v>43</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
@@ -824,10 +824,10 @@
         <v>21</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
@@ -839,9 +839,11 @@
         <v>22</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="29"/>

</xml_diff>

<commit_message>
Hoang tich hop chuc nang QuanLyLoaiDiaDiem
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>70% (Chưa có cn Cập Nhật)</t>
+  </si>
+  <si>
+    <t>75% (Làm được 3/4 chức năng)</t>
+  </si>
+  <si>
+    <t>100% (10/06/2010)</t>
   </si>
 </sst>
 </file>
@@ -364,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -447,6 +453,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,7 +751,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -875,8 +882,12 @@
       <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="D9" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="29"/>

</xml_diff>

<commit_message>
Tuan Anh hoang thanh chuc nang qlMatHang (75%).
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>100% (10/06/2010)</t>
+  </si>
+  <si>
+    <t>75%.còn phần cập nhật mặt hàng.MainForm có tí trục trặc nên sửa form lại tí</t>
   </si>
 </sst>
 </file>
@@ -423,6 +426,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -453,7 +457,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,7 +754,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -765,13 +768,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="5" t="s">
@@ -791,7 +794,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -808,7 +811,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="29"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
@@ -823,7 +826,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="29"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
@@ -838,7 +841,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="29"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
@@ -853,7 +856,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="29"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
@@ -864,7 +867,7 @@
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="29"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
@@ -875,14 +878,14 @@
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="29"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="22" t="s">
         <v>54</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -890,18 +893,20 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="9" t="s">
         <v>31</v>
       </c>
@@ -912,7 +917,7 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="29"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
@@ -923,7 +928,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="29.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -936,7 +941,7 @@
       <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="15" t="s">
         <v>8</v>
       </c>
@@ -947,7 +952,7 @@
       <c r="E14" s="14"/>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="18" t="s">
@@ -960,7 +965,7 @@
       <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
@@ -971,7 +976,7 @@
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
@@ -982,43 +987,43 @@
       <c r="E17" s="11"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="19"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="20"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="20"/>
     </row>
     <row r="24" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="20"/>
     </row>
   </sheetData>
@@ -1065,7 +1070,7 @@
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1073,13 +1078,13 @@
       <c r="A3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="32"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Hoang điều chỉnh tiến độ PhanCongDot3.xlsx thêm 2 ngày.
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -155,47 +155,14 @@
     <t>Tổng Quát</t>
   </si>
   <si>
-    <t>18h - 7/06/2011</t>
-  </si>
-  <si>
-    <t>18h - 7/06/2012</t>
-  </si>
-  <si>
-    <t>18h - 8/06/2013</t>
-  </si>
-  <si>
-    <t>18h - 8/06/2014</t>
-  </si>
-  <si>
     <t>18h - 8/06/2015</t>
   </si>
   <si>
     <t>18h - 9/06/2016</t>
-  </si>
-  <si>
-    <t>18h - 9/06/2017</t>
-  </si>
-  <si>
-    <t>18h - 9/06/2018</t>
-  </si>
-  <si>
-    <t>18h - 9/06/2019</t>
-  </si>
-  <si>
-    <t>18h - 9/06/2021</t>
   </si>
   <si>
     <t>3.11 Quản lý thông tin việc Cấp Nhiên Liệu
 - Phụ trách: Văn Hoàng</t>
-  </si>
-  <si>
-    <t>18h - 10/06/2020</t>
-  </si>
-  <si>
-    <t>18h - 10/06/2022</t>
-  </si>
-  <si>
-    <t>18h - 10/06/2023</t>
   </si>
   <si>
     <t>Kết Quả Tính Đến 
@@ -271,13 +238,133 @@
   </si>
   <si>
     <t>75%.còn phần cập nhật mặt hàng.MainForm có tí trục trặc nên sửa form lại tí</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 8/06/2010
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đc: 18h-11/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 9/06/2010
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-11/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 9/06/2018
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-11/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 9/06/2019
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-11/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 10/06/2020
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-12/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 9/06/2021
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-11/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 10/06/2022
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-12/06/2010</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">18h - 10/06/2023
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>đ/c: 18h-12/06/2010</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +388,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -373,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -397,9 +490,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -456,6 +546,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -768,13 +867,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="A1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="5" t="s">
@@ -787,244 +886,244 @@
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.25">
+      <c r="A3" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29.25">
-      <c r="A3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="30"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="30"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="30"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="30"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="C7" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="30"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="C8" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="30"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>55</v>
+      <c r="C9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="30"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="30"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>47</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="30"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>28</v>
+      <c r="C12" s="33" t="s">
+        <v>48</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="29.25">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="29"/>
+      <c r="B14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A15" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="28"/>
+      <c r="B16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17" s="28"/>
+      <c r="B17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-    </row>
-    <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="30"/>
-      <c r="B14" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A15" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="29"/>
-      <c r="B16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="29"/>
-      <c r="B17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="28" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="19"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1">
+      <c r="A23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" ht="51.75" customHeight="1">
+      <c r="A24" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="20"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="20"/>
-    </row>
-    <row r="24" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A24" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="20"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1059,32 +1158,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A1" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>37</v>
+      <c r="A1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30">
       <c r="A2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30">
       <c r="A3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="32"/>
+        <v>34</v>
+      </c>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="32"/>
+        <v>35</v>
+      </c>
+      <c r="B4" s="31"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Tích hợp chức năng phân công xe - tài xế. Long mới làm xong phần phân công (có xử lý lỗi nghiệp vũ khá kĩ). Các phần xóa, sửa, tra cứu làm không mất thời gian nhiều.
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -358,6 +358,9 @@
       </rPr>
       <t>đ/c: 18h-12/06/2010</t>
     </r>
+  </si>
+  <si>
+    <t>90%. Chỉ còn lại xóa, sửa</t>
   </si>
 </sst>
 </file>
@@ -517,6 +520,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -546,15 +558,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,13 +870,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="5" t="s">
@@ -893,7 +896,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -910,7 +913,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
@@ -925,7 +928,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="29"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
@@ -940,7 +943,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="29"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
@@ -955,29 +958,29 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="22" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="22" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="29"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
@@ -992,7 +995,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1005,124 +1008,126 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="23" t="s">
         <v>47</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="29"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="23" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="29"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="24" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="28"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="24" t="s">
         <v>52</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="28"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="24" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="18"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="19"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
       <c r="D23" s="19"/>
     </row>
     <row r="24" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="19"/>
     </row>
   </sheetData>
@@ -1169,7 +1174,7 @@
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1177,13 +1182,13 @@
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="34"/>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="34"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Hoang them chuc nang ql Dia Diem (100%)
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -361,6 +361,15 @@
   </si>
   <si>
     <t>90%. Chỉ còn lại xóa, sửa</t>
+  </si>
+  <si>
+    <t>100% (11/06/2010)</t>
+  </si>
+  <si>
+    <t>100% (17/06/2010)</t>
+  </si>
+  <si>
+    <t>100% (16/06/2010)</t>
   </si>
 </sst>
 </file>
@@ -855,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -977,7 +986,9 @@
         <v>46</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="30">
       <c r="A9" s="32"/>
@@ -1005,7 +1016,9 @@
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="30">
       <c r="A11" s="32"/>
@@ -1042,7 +1055,9 @@
       <c r="D13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30">
       <c r="A14" s="32"/>

</xml_diff>

<commit_message>
Cap nhat bang phan cong
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>100% (16/06/2010)</t>
+  </si>
+  <si>
+    <t>100%(17/06/2010)</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -568,6 +571,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -864,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,8 +1043,12 @@
       <c r="C12" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="35">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30">
       <c r="A13" s="31" t="s">

</xml_diff>

<commit_message>
Hoang cập nhật tiến độ công việc Đợt 3
</commit_message>
<xml_diff>
--- a/Process/PhanCongDot3.xlsx
+++ b/Process/PhanCongDot3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t>3.3 Quản lý thông tin Trọng Tải
 - Phụ trách: Nhất Anh</t>
@@ -222,19 +222,10 @@
     <t>75%(Chưa làm phần GUI )</t>
   </si>
   <si>
-    <t>100% (9/06/2010)</t>
-  </si>
-  <si>
-    <t>100% (8/06/2010)</t>
-  </si>
-  <si>
     <t>70% (Chưa có cn Cập Nhật)</t>
   </si>
   <si>
     <t>75% (Làm được 3/4 chức năng)</t>
-  </si>
-  <si>
-    <t>100% (10/06/2010)</t>
   </si>
   <si>
     <t>75%.còn phần cập nhật mặt hàng.MainForm có tí trục trặc nên sửa form lại tí</t>
@@ -363,23 +354,88 @@
     <t>90%. Chỉ còn lại xóa, sửa</t>
   </si>
   <si>
-    <t>100% (11/06/2010)</t>
-  </si>
-  <si>
-    <t>100% (17/06/2010)</t>
-  </si>
-  <si>
-    <t>100% (16/06/2010)</t>
-  </si>
-  <si>
-    <t>100%(17/06/2010)</t>
+    <t>Hoàn chỉnh giao diện và các chức năng còn lại</t>
+  </si>
+  <si>
+    <t>4.1 Thêm chức năng quản lý Loại Nhân Viên
+- Phụ trách: Huỳnh Trân</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>(khó khăn do không có dữ liệu)</t>
+  </si>
+  <si>
+    <t>21h - 17/06/2010</t>
+  </si>
+  <si>
+    <t>90% (còn một số lỗi nhỏ)</t>
+  </si>
+  <si>
+    <t>no (giao cho Huỳnh Trân)</t>
+  </si>
+  <si>
+    <t>12h - 18/06/2010</t>
+  </si>
+  <si>
+    <t>4.2 Cấp nhiên liệu cho xe
+- Phụ trách: Huỳnh Trân</t>
+  </si>
+  <si>
+    <t>4.3 Tổng hợp báo cáo + UserGuide
+- Phụ trách: Tuấn Anh + Nhất Anh</t>
+  </si>
+  <si>
+    <t>21 - 17/06/2010</t>
+  </si>
+  <si>
+    <t>4.4 Tạo SetUp và tổng hợp lại Code
+- Phụ trách: Lê Long</t>
+  </si>
+  <si>
+    <t>4.4 Đồng bộ giao diện, code và fix chức năng tạm
+- Phụ trách: Văn Hoàng</t>
+  </si>
+  <si>
+    <t>20h - 18/06/2010</t>
+  </si>
+  <si>
+    <t>100% (8/06/2010) - Hoàng</t>
+  </si>
+  <si>
+    <t>100% (9/06/2010) - Hoàng</t>
+  </si>
+  <si>
+    <t>100% (17/06/2010) - Hoàng</t>
+  </si>
+  <si>
+    <t>100% (10/06/2010) - Hoàng</t>
+  </si>
+  <si>
+    <t>100% (11/06/2010) - Hoàng</t>
+  </si>
+  <si>
+    <t>100%(17/06/2010) - Hoàng</t>
+  </si>
+  <si>
+    <t>100% (16/06/2010) - Lê Long</t>
+  </si>
+  <si>
+    <t>30% (1/3 chức năng) - Lê Long</t>
+  </si>
+  <si>
+    <t>100% - Hoàng</t>
+  </si>
+  <si>
+    <t>100%.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,8 +468,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,6 +529,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -481,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -516,9 +583,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -541,9 +605,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -571,7 +639,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -878,18 +958,18 @@
     <col min="2" max="2" width="44.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" ht="28.5">
       <c r="A2" s="5" t="s">
@@ -909,24 +989,24 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="29.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="32"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
@@ -934,14 +1014,14 @@
         <v>32</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="32"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
@@ -949,14 +1029,14 @@
         <v>32</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="32"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
@@ -967,50 +1047,56 @@
         <v>39</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
-      <c r="A7" s="32"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="C7" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="30">
-      <c r="A8" s="32"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="13"/>
+      <c r="C8" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="E8" s="13" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="32"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="21" t="s">
-        <v>43</v>
+      <c r="D9" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1018,152 +1104,238 @@
         <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
-      <c r="A11" s="32"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="32"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="35">
-        <v>1</v>
+      <c r="C12" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>49</v>
+      <c r="C13" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="32"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="C14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="C15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="30">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+      <c r="C16" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="31"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30">
+      <c r="A18" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="30" t="s">
+      <c r="C18" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="A19" s="38"/>
+      <c r="B19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="A20" s="38"/>
+      <c r="B20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="30">
+      <c r="A21" s="38"/>
+      <c r="B21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="A22" s="38"/>
+      <c r="B22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="25" spans="1:5" ht="30" customHeight="1">
+      <c r="A25" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="18"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="25" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="51.75" customHeight="1">
+      <c r="A26" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="26" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="19"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1">
-      <c r="A23" s="27" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" ht="51.75" customHeight="1">
-      <c r="A24" s="28" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="19"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
+  <mergeCells count="10">
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1186,10 +1358,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1197,7 +1369,7 @@
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1205,13 +1377,13 @@
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="35"/>
     </row>
     <row r="4" spans="1:2" ht="30">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="35"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1"/>

</xml_diff>